<commit_message>
Successfully Working - 27 Mar 2015
</commit_message>
<xml_diff>
--- a/XSLS/LinkedIn_Test_Cases.xlsx
+++ b/XSLS/LinkedIn_Test_Cases.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Development\LinkedIn\XSLS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="21210" windowHeight="11130" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Coversheet" sheetId="4" r:id="rId1"/>
@@ -23,12 +18,13 @@
   <definedNames>
     <definedName name="data">data!$A$1:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="378">
   <si>
     <t>Number of Test Cases</t>
   </si>
@@ -1216,60 +1212,9 @@
     <t>SignIn Module</t>
   </si>
   <si>
-    <t>0 minutes 7 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:01:31 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:01:46 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 15 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:01:55 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:02:04 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 8 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:02:13 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:02:26 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 12 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:02:41 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:02:48 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:03:06 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:03:17 IST 2014</t>
-  </si>
-  <si>
     <t>0 minutes 11 seconds</t>
   </si>
   <si>
-    <t>Wed Dec 24 14:03:27 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:03:49 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 22 seconds</t>
-  </si>
-  <si>
     <t>Wed Dec 24 14:29:55 IST 2014</t>
   </si>
   <si>
@@ -1279,624 +1224,12 @@
     <t>Automation Details</t>
   </si>
   <si>
-    <t>Wed Dec 24 14:38:19 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:38:33 IST 2014</t>
-  </si>
-  <si>
     <t>0 minutes 13 seconds</t>
   </si>
   <si>
-    <t>Wed Dec 24 14:38:42 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:38:52 IST 2014</t>
-  </si>
-  <si>
     <t>0 minutes 9 seconds</t>
   </si>
   <si>
-    <t>Wed Dec 24 14:39:01 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:39:13 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:39:21 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:39:29 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:39:38 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:39:51 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:40:00 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:40:24 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 24 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:51:03 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:51:15 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:51:27 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:51:36 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:51:45 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:51:57 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:52:08 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:52:15 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:52:25 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:52:36 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:52:46 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 14:53:08 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 21 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:02:10 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:02:21 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:02:34 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:02:45 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:02:55 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:03:02 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:03:11 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:03:22 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:03:32 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:03:54 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:08:23 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:08:34 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:09:42 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:09:56 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:11:43 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:11:59 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:12:36 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:12:49 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:14:36 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:14:49 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:16:53 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:17:07 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:23:13 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:23:30 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 16 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:40:12 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 15:40:28 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:16:12 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:16:39 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 27 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:20:10 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:20:34 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 23 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:20:53 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:21:04 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:21:16 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:21:30 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:21:41 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:21:49 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:22:06 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:22:23 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 17 seconds</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:22:33 IST 2014</t>
-  </si>
-  <si>
-    <t>Wed Dec 24 17:22:58 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 25 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:32:27 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:33:38 IST 2014</t>
-  </si>
-  <si>
-    <t>1 minutes 11 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:33:42 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:34:41 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 58 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:35:09 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:35:54 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 45 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:38:18 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:39:16 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:39:43 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:40:16 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 33 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:45:41 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:46:57 IST 2014</t>
-  </si>
-  <si>
-    <t>1 minutes 16 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:47:49 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:48:24 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 35 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:55:19 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 11:55:32 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 12:00:27 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 12:00:39 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 12:00:43 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 12:01:33 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 50 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 12:01:36 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 12:02:33 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 57 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:11:12 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:11:24 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:11:26 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:13:06 IST 2014</t>
-  </si>
-  <si>
-    <t>1 minutes 40 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:13:09 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:14:22 IST 2014</t>
-  </si>
-  <si>
-    <t>1 minutes 13 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:15:54 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:16:06 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:16:08 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:16:39 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 31 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:16:42 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:17:48 IST 2014</t>
-  </si>
-  <si>
-    <t>1 minutes 6 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:20:24 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:20:36 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:20:38 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:21:17 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 38 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:21:19 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:24:16 IST 2014</t>
-  </si>
-  <si>
-    <t>2 minutes 57 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:24:17 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:25:11 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 53 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:25:12 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:28:31 IST 2014</t>
-  </si>
-  <si>
-    <t>3 minutes 18 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:28:34 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:32:02 IST 2014</t>
-  </si>
-  <si>
-    <t>3 minutes 27 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:36:16 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:36:29 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:36:31 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:37:30 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 59 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:37:33 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:39:36 IST 2014</t>
-  </si>
-  <si>
-    <t>2 minutes 3 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:39:37 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:41:23 IST 2014</t>
-  </si>
-  <si>
-    <t>1 minutes 45 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:41:24 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:45:25 IST 2014</t>
-  </si>
-  <si>
-    <t>4 minutes 0 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:45:26 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:45:59 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:54:49 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:55:03 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:55:07 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:57:34 IST 2014</t>
-  </si>
-  <si>
-    <t>2 minutes 27 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:57:39 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:59:10 IST 2014</t>
-  </si>
-  <si>
-    <t>1 minutes 31 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:59:11 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:59:57 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 14:59:59 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:00:40 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 40 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:00:41 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:01:26 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 44 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:05:31 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:05:45 IST 2014</t>
-  </si>
-  <si>
-    <t>0 minutes 14 seconds</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:39:40 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:39:56 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:50:23 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:50:36 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:54:18 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:54:32 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:55:31 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:55:45 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:59:07 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 15:59:20 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:01:25 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:01:40 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:03:23 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:03:34 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:05:53 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:06:04 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:08:01 IST 2014</t>
-  </si>
-  <si>
-    <t>Thu Dec 25 16:08:28 IST 2014</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 11:48:39 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 11:48:51 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:56:27 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:56:42 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:56:43 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:56:56 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:56:58 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:57:12 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:57:13 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:57:24 IST 2015</t>
-  </si>
-  <si>
-    <t>0 minutes 10 seconds</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:57:25 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:57:44 IST 2015</t>
-  </si>
-  <si>
-    <t>0 minutes 18 seconds</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:57:46 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 14:58:18 IST 2015</t>
-  </si>
-  <si>
-    <t>0 minutes 32 seconds</t>
-  </si>
-  <si>
     <t>Mon Mar 23 15:41:22 IST 2015</t>
   </si>
   <si>
@@ -1924,25 +1257,25 @@
     <t>0 minutes 6 seconds</t>
   </si>
   <si>
-    <t>Mon Mar 23 15:42:48 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 15:43:12 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 15:43:21 IST 2015</t>
-  </si>
-  <si>
-    <t>Mon Mar 23 15:44:43 IST 2015</t>
-  </si>
-  <si>
-    <t>1 minutes 21 seconds</t>
+    <t>Wed Mar 25 15:33:02 IST 2015</t>
+  </si>
+  <si>
+    <t>Wed Mar 25 15:33:08 IST 2015</t>
+  </si>
+  <si>
+    <t>0 minutes 5 seconds</t>
+  </si>
+  <si>
+    <t>Wed Mar 25 15:33:09 IST 2015</t>
+  </si>
+  <si>
+    <t>Wed Mar 25 15:33:15 IST 2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2850,7 +2183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2882,10 +2215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2917,7 +2249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3093,7 +2424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3103,42 +2434,42 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="19.7109375" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="28.85546875" collapsed="true"/>
     <col min="6" max="6" customWidth="true" hidden="true" width="54.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="67"/>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
       <c r="D1" s="67"/>
       <c r="E1" s="67"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="67"/>
       <c r="D2" s="67"/>
       <c r="E2" s="67"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="67"/>
       <c r="B3" s="67"/>
       <c r="C3" s="67"/>
       <c r="D3" s="67"/>
       <c r="E3" s="67"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="67"/>
       <c r="B4" s="67"/>
       <c r="C4" s="67"/>
       <c r="D4" s="67"/>
       <c r="E4" s="67"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="36" t="s">
         <v>176</v>
       </c>
@@ -3149,7 +2480,7 @@
       <c r="D5" s="68"/>
       <c r="E5" s="68"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="36" t="s">
         <v>177</v>
       </c>
@@ -3160,7 +2491,7 @@
       <c r="D6" s="68"/>
       <c r="E6" s="68"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="36" t="s">
         <v>179</v>
       </c>
@@ -3171,7 +2502,7 @@
       <c r="D7" s="68"/>
       <c r="E7" s="68"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="36" t="s">
         <v>180</v>
       </c>
@@ -3182,7 +2513,7 @@
       <c r="D8" s="70"/>
       <c r="E8" s="70"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
         <v>181</v>
       </c>
@@ -3193,13 +2524,13 @@
       <c r="D9" s="66"/>
       <c r="E9" s="66"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="37"/>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -3215,7 +2546,7 @@
     <mergeCell ref="B8:E8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId21"/>
+    <hyperlink ref="B8" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3224,7 +2555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3234,7 +2565,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="13.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="true"/>
@@ -3244,7 +2575,7 @@
     <col min="6" max="6" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75">
       <c r="A1" s="71" t="s">
         <v>226</v>
       </c>
@@ -3254,7 +2585,7 @@
       <c r="E1" s="72"/>
       <c r="F1" s="72"/>
     </row>
-    <row r="2" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="32.25" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>227</v>
       </c>
@@ -3274,7 +2605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="39">
         <v>1</v>
       </c>
@@ -3283,22 +2614,22 @@
       </c>
       <c r="C3" s="13">
         <f>'Sign In'!B64</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="13">
         <f>'Sign In'!B61</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="13">
         <f>'Sign In'!B62</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="13">
         <f>'Sign In'!B63</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="39">
         <v>2</v>
       </c>
@@ -3322,7 +2653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="39">
         <v>3</v>
       </c>
@@ -3346,26 +2677,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="15"/>
       <c r="B6" s="40" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="14">
         <f>SUM(C3:C5)</f>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="14">
         <f>SUM(D3,D5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="14">
         <f>SUM(E3,E5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="14">
         <f>SUM(F3:F5)</f>
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3377,7 +2708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3388,7 +2719,7 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="8" width="54.85546875" collapsed="true"/>
@@ -3401,7 +2732,7 @@
     <col min="9" max="9" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="49.5" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -3430,7 +2761,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="25.5">
       <c r="A2" s="52" t="s">
         <v>243</v>
       </c>
@@ -3459,7 +2790,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="38.25">
       <c r="A3" s="52" t="s">
         <v>244</v>
       </c>
@@ -3488,7 +2819,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="38.25">
       <c r="A4" s="52" t="s">
         <v>245</v>
       </c>
@@ -3511,7 +2842,7 @@
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
     </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="38.25">
       <c r="A5" s="52" t="s">
         <v>246</v>
       </c>
@@ -3534,7 +2865,7 @@
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
     </row>
-    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="38.25">
       <c r="A6" s="52" t="s">
         <v>247</v>
       </c>
@@ -3557,7 +2888,7 @@
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
     </row>
-    <row r="7" spans="1:9" s="45" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="45" customFormat="1" ht="38.25">
       <c r="A7" s="52" t="s">
         <v>248</v>
       </c>
@@ -3580,7 +2911,7 @@
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
     </row>
-    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="38.25">
       <c r="A8" s="52" t="s">
         <v>249</v>
       </c>
@@ -3603,7 +2934,7 @@
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
     </row>
-    <row r="9" spans="1:9" s="45" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="45" customFormat="1" ht="38.25">
       <c r="A9" s="52" t="s">
         <v>250</v>
       </c>
@@ -3626,7 +2957,7 @@
       <c r="H9" s="44"/>
       <c r="I9" s="44"/>
     </row>
-    <row r="10" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="76.5">
       <c r="A10" s="52" t="s">
         <v>251</v>
       </c>
@@ -3649,7 +2980,7 @@
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
     </row>
-    <row r="11" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="89.25">
       <c r="A11" s="52" t="s">
         <v>252</v>
       </c>
@@ -3672,7 +3003,7 @@
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
     </row>
-    <row r="12" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="76.5">
       <c r="A12" s="52" t="s">
         <v>253</v>
       </c>
@@ -3695,7 +3026,7 @@
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
     </row>
-    <row r="13" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="76.5">
       <c r="A13" s="52" t="s">
         <v>254</v>
       </c>
@@ -3718,7 +3049,7 @@
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
     </row>
-    <row r="14" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="89.25">
       <c r="A14" s="52" t="s">
         <v>255</v>
       </c>
@@ -3741,7 +3072,7 @@
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
     </row>
-    <row r="15" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="89.25">
       <c r="A15" s="52" t="s">
         <v>256</v>
       </c>
@@ -3764,7 +3095,7 @@
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
-    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="51">
       <c r="A16" s="52" t="s">
         <v>257</v>
       </c>
@@ -3787,7 +3118,7 @@
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="51">
       <c r="A17" s="52" t="s">
         <v>258</v>
       </c>
@@ -3810,7 +3141,7 @@
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="38.25">
       <c r="A18" s="52" t="s">
         <v>259</v>
       </c>
@@ -3833,7 +3164,7 @@
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="76.5">
       <c r="A19" s="52" t="s">
         <v>260</v>
       </c>
@@ -3856,7 +3187,7 @@
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="76.5">
       <c r="A20" s="52" t="s">
         <v>261</v>
       </c>
@@ -3879,7 +3210,7 @@
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="76.5">
       <c r="A21" s="52" t="s">
         <v>262</v>
       </c>
@@ -3902,7 +3233,7 @@
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="76.5">
       <c r="A22" s="52" t="s">
         <v>263</v>
       </c>
@@ -3925,7 +3256,7 @@
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="76.5">
       <c r="A23" s="52" t="s">
         <v>264</v>
       </c>
@@ -3948,7 +3279,7 @@
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
     </row>
-    <row r="24" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="76.5">
       <c r="A24" s="52" t="s">
         <v>265</v>
       </c>
@@ -3971,7 +3302,7 @@
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="76.5">
       <c r="A25" s="52" t="s">
         <v>266</v>
       </c>
@@ -3994,7 +3325,7 @@
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
     </row>
-    <row r="26" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="76.5">
       <c r="A26" s="52" t="s">
         <v>267</v>
       </c>
@@ -4017,7 +3348,7 @@
       <c r="H26" s="29"/>
       <c r="I26" s="29"/>
     </row>
-    <row r="27" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="76.5">
       <c r="A27" s="52" t="s">
         <v>268</v>
       </c>
@@ -4040,7 +3371,7 @@
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="76.5">
       <c r="A28" s="52" t="s">
         <v>269</v>
       </c>
@@ -4063,7 +3394,7 @@
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="76.5">
       <c r="A29" s="52" t="s">
         <v>270</v>
       </c>
@@ -4086,7 +3417,7 @@
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="76.5">
       <c r="A30" s="52" t="s">
         <v>271</v>
       </c>
@@ -4109,7 +3440,7 @@
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
     </row>
-    <row r="31" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="76.5">
       <c r="A31" s="52" t="s">
         <v>272</v>
       </c>
@@ -4132,7 +3463,7 @@
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
     </row>
-    <row r="32" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="76.5">
       <c r="A32" s="52" t="s">
         <v>273</v>
       </c>
@@ -4155,7 +3486,7 @@
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
     </row>
-    <row r="33" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="76.5">
       <c r="A33" s="52" t="s">
         <v>274</v>
       </c>
@@ -4178,7 +3509,7 @@
       <c r="H33" s="29"/>
       <c r="I33" s="29"/>
     </row>
-    <row r="34" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="76.5">
       <c r="A34" s="52" t="s">
         <v>275</v>
       </c>
@@ -4201,7 +3532,7 @@
       <c r="H34" s="29"/>
       <c r="I34" s="29"/>
     </row>
-    <row r="35" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="63.75">
       <c r="A35" s="52" t="s">
         <v>276</v>
       </c>
@@ -4224,7 +3555,7 @@
       <c r="H35" s="29"/>
       <c r="I35" s="29"/>
     </row>
-    <row r="36" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="76.5">
       <c r="A36" s="52" t="s">
         <v>277</v>
       </c>
@@ -4247,7 +3578,7 @@
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
     </row>
-    <row r="37" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="76.5">
       <c r="A37" s="52" t="s">
         <v>278</v>
       </c>
@@ -4270,7 +3601,7 @@
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
     </row>
-    <row r="38" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="76.5">
       <c r="A38" s="52" t="s">
         <v>279</v>
       </c>
@@ -4293,7 +3624,7 @@
       <c r="H38" s="29"/>
       <c r="I38" s="29"/>
     </row>
-    <row r="39" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="76.5">
       <c r="A39" s="52" t="s">
         <v>280</v>
       </c>
@@ -4316,7 +3647,7 @@
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
     </row>
-    <row r="40" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="63.75">
       <c r="A40" s="52" t="s">
         <v>281</v>
       </c>
@@ -4339,7 +3670,7 @@
       <c r="H40" s="29"/>
       <c r="I40" s="29"/>
     </row>
-    <row r="41" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="76.5">
       <c r="A41" s="52" t="s">
         <v>282</v>
       </c>
@@ -4362,7 +3693,7 @@
       <c r="H41" s="29"/>
       <c r="I41" s="29"/>
     </row>
-    <row r="42" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="76.5">
       <c r="A42" s="52" t="s">
         <v>283</v>
       </c>
@@ -4385,7 +3716,7 @@
       <c r="H42" s="29"/>
       <c r="I42" s="29"/>
     </row>
-    <row r="43" spans="1:9" s="45" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="45" customFormat="1" ht="63.75">
       <c r="A43" s="52" t="s">
         <v>284</v>
       </c>
@@ -4408,7 +3739,7 @@
       <c r="H43" s="44"/>
       <c r="I43" s="44"/>
     </row>
-    <row r="44" spans="1:9" s="45" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="45" customFormat="1" ht="102">
       <c r="A44" s="52" t="s">
         <v>285</v>
       </c>
@@ -4431,7 +3762,7 @@
       <c r="H44" s="44"/>
       <c r="I44" s="44"/>
     </row>
-    <row r="45" spans="1:9" s="45" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="45" customFormat="1" ht="76.5">
       <c r="A45" s="52" t="s">
         <v>286</v>
       </c>
@@ -4454,7 +3785,7 @@
       <c r="H45" s="44"/>
       <c r="I45" s="44"/>
     </row>
-    <row r="46" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="76.5">
       <c r="A46" s="52" t="s">
         <v>287</v>
       </c>
@@ -4477,7 +3808,7 @@
       <c r="H46" s="29"/>
       <c r="I46" s="29"/>
     </row>
-    <row r="47" spans="1:9" s="50" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="50" customFormat="1" ht="38.25">
       <c r="A47" s="52" t="s">
         <v>288</v>
       </c>
@@ -4500,7 +3831,7 @@
       <c r="H47" s="49"/>
       <c r="I47" s="49"/>
     </row>
-    <row r="48" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="38.25">
       <c r="A48" s="52" t="s">
         <v>289</v>
       </c>
@@ -4523,7 +3854,7 @@
       <c r="H48" s="29"/>
       <c r="I48" s="29"/>
     </row>
-    <row r="49" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="51">
       <c r="A49" s="52" t="s">
         <v>290</v>
       </c>
@@ -4546,7 +3877,7 @@
       <c r="H49" s="29"/>
       <c r="I49" s="29"/>
     </row>
-    <row r="50" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="25.5">
       <c r="A50" s="52" t="s">
         <v>291</v>
       </c>
@@ -4569,7 +3900,7 @@
       <c r="H50" s="31"/>
       <c r="I50" s="31"/>
     </row>
-    <row r="51" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="25.5">
       <c r="A51" s="52" t="s">
         <v>292</v>
       </c>
@@ -4592,7 +3923,7 @@
       <c r="H51" s="31"/>
       <c r="I51" s="31"/>
     </row>
-    <row r="52" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="25.5">
       <c r="A52" s="52" t="s">
         <v>293</v>
       </c>
@@ -4615,67 +3946,67 @@
       <c r="H52" s="31"/>
       <c r="I52" s="31"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="7"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="7"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="7"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="73" t="s">
         <v>64</v>
       </c>
       <c r="B60" s="73"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="17">
         <f>COUNTIF(F2:F25,"Pass")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B62" s="19">
         <f>COUNTIF(F2:F25,"Fail")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B63" s="21">
         <f>COUNTIF(F2:F25,"Not Tested")</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.75">
       <c r="A64" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="22">
         <f>SUM(B61,B63)</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -4704,17 +4035,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="21.42578125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="54.28515625" collapsed="true"/>
@@ -4727,7 +4058,7 @@
     <col min="9" max="11" customWidth="true" width="28.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="54" t="s">
         <v>303</v>
       </c>
@@ -4741,20 +4072,22 @@
       <c r="E1" s="56">
         <v>0</v>
       </c>
-      <c r="F1" s="77"/>
+      <c r="F1" s="77" t="s">
+        <v>8</v>
+      </c>
       <c r="G1" s="78"/>
       <c r="H1" s="79"/>
       <c r="I1" s="80" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="J1" s="81" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
       <c r="K1" s="82" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="54" t="s">
         <v>305</v>
       </c>
@@ -4775,7 +4108,7 @@
       <c r="J2" s="84"/>
       <c r="K2" s="85"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="54" t="s">
         <v>307</v>
       </c>
@@ -4796,7 +4129,7 @@
       <c r="J3" s="84"/>
       <c r="K3" s="85"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="54" t="s">
         <v>310</v>
       </c>
@@ -4817,7 +4150,7 @@
       <c r="J4" s="84"/>
       <c r="K4" s="85"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="58" t="s">
         <v>311</v>
       </c>
@@ -4834,7 +4167,7 @@
       <c r="J5" s="87"/>
       <c r="K5" s="88"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="74"/>
       <c r="B6" s="75"/>
       <c r="C6" s="75"/>
@@ -4847,7 +4180,7 @@
       <c r="J6" s="75"/>
       <c r="K6" s="76"/>
     </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="75">
       <c r="A7" s="60" t="s">
         <v>312</v>
       </c>
@@ -4882,7 +4215,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="25.5">
       <c r="A8" s="52" t="s">
         <v>243</v>
       </c>
@@ -4904,16 +4237,16 @@
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="65" t="s">
-        <v>585</v>
+        <v>364</v>
       </c>
       <c r="J8" s="65" t="s">
-        <v>586</v>
+        <v>365</v>
       </c>
       <c r="K8" s="65" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="25.5">
       <c r="A9" s="52" t="s">
         <v>244</v>
       </c>
@@ -4935,16 +4268,16 @@
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="65" t="s">
-        <v>587</v>
+        <v>366</v>
       </c>
       <c r="J9" s="65" t="s">
-        <v>588</v>
+        <v>367</v>
       </c>
       <c r="K9" s="65" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="25.5">
       <c r="A10" s="52" t="s">
         <v>245</v>
       </c>
@@ -4966,16 +4299,16 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="65" t="s">
-        <v>589</v>
+        <v>368</v>
       </c>
       <c r="J10" s="65" t="s">
-        <v>590</v>
+        <v>369</v>
       </c>
       <c r="K10" s="65" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="25.5">
       <c r="A11" s="52" t="s">
         <v>246</v>
       </c>
@@ -4997,16 +4330,16 @@
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
       <c r="I11" s="65" t="s">
-        <v>591</v>
+        <v>370</v>
       </c>
       <c r="J11" s="65" t="s">
-        <v>592</v>
+        <v>371</v>
       </c>
       <c r="K11" s="65" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5">
       <c r="A12" s="52" t="s">
         <v>247</v>
       </c>
@@ -5028,16 +4361,16 @@
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
       <c r="I12" s="65" t="s">
-        <v>594</v>
+        <v>373</v>
       </c>
       <c r="J12" s="65" t="s">
-        <v>595</v>
+        <v>374</v>
       </c>
       <c r="K12" s="65" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="38.25">
       <c r="A13" s="52" t="s">
         <v>248</v>
       </c>
@@ -5062,7 +4395,7 @@
       <c r="J13" s="65"/>
       <c r="K13" s="65"/>
     </row>
-    <row r="14" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="25.5">
       <c r="A14" s="52" t="s">
         <v>249</v>
       </c>
@@ -5084,16 +4417,16 @@
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
       <c r="I14" s="65" t="s">
-        <v>596</v>
+        <v>376</v>
       </c>
       <c r="J14" s="65" t="s">
-        <v>597</v>
+        <v>377</v>
       </c>
       <c r="K14" s="65" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="25.5">
       <c r="A15" s="52" t="s">
         <v>250</v>
       </c>
@@ -5110,7 +4443,7 @@
         <v>96</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
@@ -5118,7 +4451,7 @@
       <c r="J15" s="65"/>
       <c r="K15" s="65"/>
     </row>
-    <row r="16" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="63.75">
       <c r="A16" s="52" t="s">
         <v>251</v>
       </c>
@@ -5135,7 +4468,7 @@
         <v>121</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
@@ -5143,7 +4476,7 @@
       <c r="J16" s="65"/>
       <c r="K16" s="65"/>
     </row>
-    <row r="17" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="63.75">
       <c r="A17" s="52" t="s">
         <v>252</v>
       </c>
@@ -5160,7 +4493,7 @@
         <v>123</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
@@ -5168,7 +4501,7 @@
       <c r="J17" s="65"/>
       <c r="K17" s="65"/>
     </row>
-    <row r="18" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="63.75">
       <c r="A18" s="52" t="s">
         <v>253</v>
       </c>
@@ -5185,7 +4518,7 @@
         <v>121</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
@@ -5193,7 +4526,7 @@
       <c r="J18" s="65"/>
       <c r="K18" s="65"/>
     </row>
-    <row r="19" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="63.75">
       <c r="A19" s="52" t="s">
         <v>254</v>
       </c>
@@ -5210,7 +4543,7 @@
         <v>126</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
@@ -5218,7 +4551,7 @@
       <c r="J19" s="65"/>
       <c r="K19" s="65"/>
     </row>
-    <row r="20" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="63.75">
       <c r="A20" s="52" t="s">
         <v>255</v>
       </c>
@@ -5243,7 +4576,7 @@
       <c r="J20" s="65"/>
       <c r="K20" s="65"/>
     </row>
-    <row r="21" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="63.75">
       <c r="A21" s="52" t="s">
         <v>256</v>
       </c>
@@ -5268,7 +4601,7 @@
       <c r="J21" s="65"/>
       <c r="K21" s="65"/>
     </row>
-    <row r="22" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="51">
       <c r="A22" s="52" t="s">
         <v>257</v>
       </c>
@@ -5293,7 +4626,7 @@
       <c r="J22" s="65"/>
       <c r="K22" s="65"/>
     </row>
-    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="51">
       <c r="A23" s="52" t="s">
         <v>258</v>
       </c>
@@ -5318,7 +4651,7 @@
       <c r="J23" s="65"/>
       <c r="K23" s="65"/>
     </row>
-    <row r="24" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="38.25">
       <c r="A24" s="52" t="s">
         <v>259</v>
       </c>
@@ -5343,7 +4676,7 @@
       <c r="J24" s="65"/>
       <c r="K24" s="65"/>
     </row>
-    <row r="25" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="76.5">
       <c r="A25" s="52" t="s">
         <v>260</v>
       </c>
@@ -5368,7 +4701,7 @@
       <c r="J25" s="65"/>
       <c r="K25" s="65"/>
     </row>
-    <row r="26" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="76.5">
       <c r="A26" s="52" t="s">
         <v>261</v>
       </c>
@@ -5393,7 +4726,7 @@
       <c r="J26" s="65"/>
       <c r="K26" s="65"/>
     </row>
-    <row r="27" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="76.5">
       <c r="A27" s="52" t="s">
         <v>262</v>
       </c>
@@ -5418,7 +4751,7 @@
       <c r="J27" s="65"/>
       <c r="K27" s="65"/>
     </row>
-    <row r="28" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="76.5">
       <c r="A28" s="52" t="s">
         <v>263</v>
       </c>
@@ -5443,7 +4776,7 @@
       <c r="J28" s="65"/>
       <c r="K28" s="65"/>
     </row>
-    <row r="29" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="76.5">
       <c r="A29" s="52" t="s">
         <v>264</v>
       </c>
@@ -5468,7 +4801,7 @@
       <c r="J29" s="65"/>
       <c r="K29" s="65"/>
     </row>
-    <row r="30" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="76.5">
       <c r="A30" s="52" t="s">
         <v>265</v>
       </c>
@@ -5493,7 +4826,7 @@
       <c r="J30" s="65"/>
       <c r="K30" s="65"/>
     </row>
-    <row r="31" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="76.5">
       <c r="A31" s="52" t="s">
         <v>266</v>
       </c>
@@ -5518,7 +4851,7 @@
       <c r="J31" s="65"/>
       <c r="K31" s="65"/>
     </row>
-    <row r="32" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="76.5">
       <c r="A32" s="52" t="s">
         <v>267</v>
       </c>
@@ -5543,7 +4876,7 @@
       <c r="J32" s="65"/>
       <c r="K32" s="65"/>
     </row>
-    <row r="33" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="76.5">
       <c r="A33" s="52" t="s">
         <v>268</v>
       </c>
@@ -5568,7 +4901,7 @@
       <c r="J33" s="65"/>
       <c r="K33" s="65"/>
     </row>
-    <row r="34" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="76.5">
       <c r="A34" s="52" t="s">
         <v>269</v>
       </c>
@@ -5593,7 +4926,7 @@
       <c r="J34" s="65"/>
       <c r="K34" s="65"/>
     </row>
-    <row r="35" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="76.5">
       <c r="A35" s="52" t="s">
         <v>270</v>
       </c>
@@ -5618,7 +4951,7 @@
       <c r="J35" s="65"/>
       <c r="K35" s="65"/>
     </row>
-    <row r="36" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="76.5">
       <c r="A36" s="52" t="s">
         <v>271</v>
       </c>
@@ -5643,7 +4976,7 @@
       <c r="J36" s="65"/>
       <c r="K36" s="65"/>
     </row>
-    <row r="37" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="76.5">
       <c r="A37" s="52" t="s">
         <v>272</v>
       </c>
@@ -5668,7 +5001,7 @@
       <c r="J37" s="65"/>
       <c r="K37" s="65"/>
     </row>
-    <row r="38" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="76.5">
       <c r="A38" s="52" t="s">
         <v>273</v>
       </c>
@@ -5693,7 +5026,7 @@
       <c r="J38" s="65"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="76.5">
       <c r="A39" s="52" t="s">
         <v>274</v>
       </c>
@@ -5718,7 +5051,7 @@
       <c r="J39" s="65"/>
       <c r="K39" s="65"/>
     </row>
-    <row r="40" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="76.5">
       <c r="A40" s="52" t="s">
         <v>275</v>
       </c>
@@ -5743,7 +5076,7 @@
       <c r="J40" s="65"/>
       <c r="K40" s="65"/>
     </row>
-    <row r="41" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="63.75">
       <c r="A41" s="52" t="s">
         <v>276</v>
       </c>
@@ -5768,7 +5101,7 @@
       <c r="J41" s="65"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="76.5">
       <c r="A42" s="52" t="s">
         <v>277</v>
       </c>
@@ -5793,7 +5126,7 @@
       <c r="J42" s="65"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="76.5">
       <c r="A43" s="52" t="s">
         <v>278</v>
       </c>
@@ -5818,7 +5151,7 @@
       <c r="J43" s="65"/>
       <c r="K43" s="65"/>
     </row>
-    <row r="44" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="76.5">
       <c r="A44" s="52" t="s">
         <v>279</v>
       </c>
@@ -5843,7 +5176,7 @@
       <c r="J44" s="65"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="76.5">
       <c r="A45" s="52" t="s">
         <v>280</v>
       </c>
@@ -5868,7 +5201,7 @@
       <c r="J45" s="65"/>
       <c r="K45" s="65"/>
     </row>
-    <row r="46" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="63.75">
       <c r="A46" s="52" t="s">
         <v>281</v>
       </c>
@@ -5893,7 +5226,7 @@
       <c r="J46" s="65"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="76.5">
       <c r="A47" s="52" t="s">
         <v>282</v>
       </c>
@@ -5918,7 +5251,7 @@
       <c r="J47" s="65"/>
       <c r="K47" s="65"/>
     </row>
-    <row r="48" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="76.5">
       <c r="A48" s="52" t="s">
         <v>283</v>
       </c>
@@ -5943,7 +5276,7 @@
       <c r="J48" s="65"/>
       <c r="K48" s="65"/>
     </row>
-    <row r="49" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="63.75">
       <c r="A49" s="52" t="s">
         <v>284</v>
       </c>
@@ -5968,7 +5301,7 @@
       <c r="J49" s="65"/>
       <c r="K49" s="65"/>
     </row>
-    <row r="50" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="89.25">
       <c r="A50" s="52" t="s">
         <v>285</v>
       </c>
@@ -5993,7 +5326,7 @@
       <c r="J50" s="65"/>
       <c r="K50" s="65"/>
     </row>
-    <row r="51" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="76.5">
       <c r="A51" s="52" t="s">
         <v>286</v>
       </c>
@@ -6018,7 +5351,7 @@
       <c r="J51" s="65"/>
       <c r="K51" s="65"/>
     </row>
-    <row r="52" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="76.5">
       <c r="A52" s="52" t="s">
         <v>287</v>
       </c>
@@ -6043,7 +5376,7 @@
       <c r="J52" s="65"/>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="38.25">
       <c r="A53" s="52" t="s">
         <v>288</v>
       </c>
@@ -6068,7 +5401,7 @@
       <c r="J53" s="65"/>
       <c r="K53" s="65"/>
     </row>
-    <row r="54" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="38.25">
       <c r="A54" s="52" t="s">
         <v>289</v>
       </c>
@@ -6093,7 +5426,7 @@
       <c r="J54" s="65"/>
       <c r="K54" s="65"/>
     </row>
-    <row r="55" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="51">
       <c r="A55" s="52" t="s">
         <v>290</v>
       </c>
@@ -6118,7 +5451,7 @@
       <c r="J55" s="65"/>
       <c r="K55" s="65"/>
     </row>
-    <row r="56" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="25.5">
       <c r="A56" s="52" t="s">
         <v>291</v>
       </c>
@@ -6143,7 +5476,7 @@
       <c r="J56" s="65"/>
       <c r="K56" s="65"/>
     </row>
-    <row r="57" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="25.5">
       <c r="A57" s="52" t="s">
         <v>292</v>
       </c>
@@ -6168,7 +5501,7 @@
       <c r="J57" s="65"/>
       <c r="K57" s="65"/>
     </row>
-    <row r="58" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="25.5">
       <c r="A58" s="52" t="s">
         <v>293</v>
       </c>
@@ -6221,7 +5554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6233,7 +5566,7 @@
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="2" width="55.0" collapsed="true"/>
@@ -6245,7 +5578,7 @@
     <col min="8" max="8" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="54" customHeight="1">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -6271,7 +5604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="25.5">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -6293,7 +5626,7 @@
       <c r="G2" s="24"/>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="25.5">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -6315,7 +5648,7 @@
       <c r="G3" s="24"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="38.25">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -6337,7 +5670,7 @@
       <c r="G4" s="24"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="25.5">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -6359,7 +5692,7 @@
       <c r="G5" s="24"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="25.5">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -6381,7 +5714,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="25.5">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -6403,7 +5736,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="25.5">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -6425,7 +5758,7 @@
       <c r="G8" s="24"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="38.25">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -6447,7 +5780,7 @@
       <c r="G9" s="24"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="38.25">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -6469,7 +5802,7 @@
       <c r="G10" s="24"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="51">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -6491,7 +5824,7 @@
       <c r="G11" s="24"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="51">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -6513,7 +5846,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="51">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -6535,7 +5868,7 @@
       <c r="G13" s="24"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="51">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -6557,7 +5890,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="51">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -6579,7 +5912,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="51">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -6601,7 +5934,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="51">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -6623,7 +5956,7 @@
       <c r="G17" s="24"/>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="51">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -6645,7 +5978,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="51">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -6667,7 +6000,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="51">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -6689,7 +6022,7 @@
       <c r="G20" s="24"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="51">
       <c r="A21" s="23">
         <v>20</v>
       </c>
@@ -6711,7 +6044,7 @@
       <c r="G21" s="24"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="51">
       <c r="A22" s="23">
         <v>21</v>
       </c>
@@ -6733,7 +6066,7 @@
       <c r="G22" s="24"/>
       <c r="H22" s="26"/>
     </row>
-    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="51">
       <c r="A23" s="23">
         <v>22</v>
       </c>
@@ -6755,7 +6088,7 @@
       <c r="G23" s="24"/>
       <c r="H23" s="26"/>
     </row>
-    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="51">
       <c r="A24" s="23">
         <v>23</v>
       </c>
@@ -6777,7 +6110,7 @@
       <c r="G24" s="24"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="51">
       <c r="A25" s="23">
         <v>24</v>
       </c>
@@ -6799,7 +6132,7 @@
       <c r="G25" s="24"/>
       <c r="H25" s="26"/>
     </row>
-    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="51">
       <c r="A26" s="23">
         <v>25</v>
       </c>
@@ -6821,7 +6154,7 @@
       <c r="G26" s="24"/>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:8" ht="102" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="102">
       <c r="A27" s="23">
         <v>26</v>
       </c>
@@ -6843,7 +6176,7 @@
       <c r="G27" s="24"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="38.25">
       <c r="A28" s="23">
         <v>27</v>
       </c>
@@ -6865,7 +6198,7 @@
       <c r="G28" s="24"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="51">
       <c r="A29" s="23">
         <v>28</v>
       </c>
@@ -6887,7 +6220,7 @@
       <c r="G29" s="24"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="51">
       <c r="A30" s="23">
         <v>29</v>
       </c>
@@ -6909,7 +6242,7 @@
       <c r="G30" s="24"/>
       <c r="H30" s="26"/>
     </row>
-    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="51">
       <c r="A31" s="23">
         <v>30</v>
       </c>
@@ -6931,7 +6264,7 @@
       <c r="G31" s="24"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="25.5">
       <c r="A32" s="23">
         <v>31</v>
       </c>
@@ -6953,7 +6286,7 @@
       <c r="G32" s="24"/>
       <c r="H32" s="26"/>
     </row>
-    <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="51">
       <c r="A33" s="23">
         <v>32</v>
       </c>
@@ -6975,7 +6308,7 @@
       <c r="G33" s="24"/>
       <c r="H33" s="26"/>
     </row>
-    <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="51">
       <c r="A34" s="23">
         <v>33</v>
       </c>
@@ -6997,7 +6330,7 @@
       <c r="G34" s="24"/>
       <c r="H34" s="26"/>
     </row>
-    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="25.5">
       <c r="A35" s="23">
         <v>34</v>
       </c>
@@ -7019,7 +6352,7 @@
       <c r="G35" s="24"/>
       <c r="H35" s="26"/>
     </row>
-    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="25.5">
       <c r="A36" s="23">
         <v>35</v>
       </c>
@@ -7041,7 +6374,7 @@
       <c r="G36" s="24"/>
       <c r="H36" s="26"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="5"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7051,7 +6384,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="5"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -7061,7 +6394,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="5"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -7071,7 +6404,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -7081,7 +6414,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15" customHeight="1">
       <c r="A41" s="89" t="s">
         <v>64</v>
       </c>
@@ -7092,7 +6425,7 @@
       <c r="F41" s="4"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="16.5" customHeight="1">
       <c r="A42" s="16" t="s">
         <v>7</v>
       </c>
@@ -7106,7 +6439,7 @@
       <c r="F42" s="4"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="14.25" customHeight="1">
       <c r="A43" s="18" t="s">
         <v>8</v>
       </c>
@@ -7120,7 +6453,7 @@
       <c r="F43" s="4"/>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1">
       <c r="A44" s="20" t="s">
         <v>9</v>
       </c>
@@ -7134,7 +6467,7 @@
       <c r="F44" s="4"/>
       <c r="G44"/>
     </row>
-    <row r="45" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="16.5" customHeight="1">
       <c r="A45" s="22" t="s">
         <v>65</v>
       </c>
@@ -7148,7 +6481,7 @@
       <c r="F45" s="4"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="2"/>
       <c r="D46" s="6"/>
       <c r="F46"/>
@@ -7180,7 +6513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -7191,7 +6524,7 @@
       <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="18.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="54.85546875" collapsed="true"/>
@@ -7202,7 +6535,7 @@
     <col min="8" max="8" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="47.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -7228,7 +6561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="25.5">
       <c r="A2" s="32">
         <v>1</v>
       </c>
@@ -7250,7 +6583,7 @@
       <c r="G2" s="34"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="38.25">
       <c r="A3" s="32">
         <v>2</v>
       </c>
@@ -7272,7 +6605,7 @@
       <c r="G3" s="34"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="25.5">
       <c r="A4" s="32">
         <v>3</v>
       </c>
@@ -7294,7 +6627,7 @@
       <c r="G4" s="34"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="25.5">
       <c r="A5" s="32">
         <v>4</v>
       </c>
@@ -7316,7 +6649,7 @@
       <c r="G5" s="34"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="25.5">
       <c r="A6" s="32">
         <v>5</v>
       </c>
@@ -7338,7 +6671,7 @@
       <c r="G6" s="34"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="25.5">
       <c r="A7" s="32">
         <v>6</v>
       </c>
@@ -7360,7 +6693,7 @@
       <c r="G7" s="34"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="38.25">
       <c r="A8" s="32">
         <v>7</v>
       </c>
@@ -7382,7 +6715,7 @@
       <c r="G8" s="34"/>
       <c r="H8" s="31"/>
     </row>
-    <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="38.25">
       <c r="A9" s="32">
         <v>8</v>
       </c>
@@ -7404,7 +6737,7 @@
       <c r="G9" s="34"/>
       <c r="H9" s="31"/>
     </row>
-    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="25.5">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -7426,7 +6759,7 @@
       <c r="G10" s="34"/>
       <c r="H10" s="31"/>
     </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="51">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -7448,7 +6781,7 @@
       <c r="G11" s="34"/>
       <c r="H11" s="31"/>
     </row>
-    <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="38.25">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -7470,7 +6803,7 @@
       <c r="G12" s="34"/>
       <c r="H12" s="31"/>
     </row>
-    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="25.5">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -7492,7 +6825,7 @@
       <c r="G13" s="34"/>
       <c r="H13" s="31"/>
     </row>
-    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="25.5">
       <c r="A14" s="32">
         <v>13</v>
       </c>
@@ -7514,7 +6847,7 @@
       <c r="G14" s="34"/>
       <c r="H14" s="31"/>
     </row>
-    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="25.5">
       <c r="A15" s="32">
         <v>14</v>
       </c>
@@ -7536,7 +6869,7 @@
       <c r="G15" s="34"/>
       <c r="H15" s="31"/>
     </row>
-    <row r="16" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="63.75">
       <c r="A16" s="32">
         <v>15</v>
       </c>
@@ -7558,16 +6891,16 @@
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="10"/>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.75">
       <c r="A20" s="73" t="s">
         <v>64</v>
       </c>
       <c r="B20" s="73"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="16" t="s">
         <v>7</v>
       </c>
@@ -7576,7 +6909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="18" t="s">
         <v>8</v>
       </c>
@@ -7585,7 +6918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="20" t="s">
         <v>9</v>
       </c>
@@ -7594,7 +6927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.75">
       <c r="A24" s="22" t="s">
         <v>65</v>
       </c>
@@ -7639,7 +6972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
@@ -7647,22 +6980,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Commit on 02 Apr 2015 - Register Successful
</commit_message>
<xml_diff>
--- a/XSLS/LinkedIn_Test_Cases.xlsx
+++ b/XSLS/LinkedIn_Test_Cases.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="378">
   <si>
     <t>Number of Test Cases</t>
   </si>
@@ -2545,7 +2545,7 @@
     <mergeCell ref="B8:E8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId35"/>
+    <hyperlink ref="B8" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -5142,7 +5142,7 @@
         <v>84</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
@@ -5167,7 +5167,7 @@
         <v>84</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
@@ -5192,7 +5192,7 @@
         <v>85</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
@@ -5217,7 +5217,7 @@
         <v>88</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
@@ -5242,7 +5242,7 @@
         <v>89</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G47" s="31"/>
       <c r="H47" s="31"/>
@@ -5267,7 +5267,7 @@
         <v>92</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G48" s="31"/>
       <c r="H48" s="31"/>
@@ -5367,7 +5367,7 @@
         <v>111</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G52" s="31"/>
       <c r="H52" s="31"/>

</xml_diff>

<commit_message>
Successfully Working - 02 Apr 2015
</commit_message>
<xml_diff>
--- a/XSLS/LinkedIn_Test_Cases.xlsx
+++ b/XSLS/LinkedIn_Test_Cases.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="378">
   <si>
     <t>Number of Test Cases</t>
   </si>
@@ -2545,7 +2545,7 @@
     <mergeCell ref="B8:E8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId55"/>
+    <hyperlink ref="B8" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>